<commit_message>
modelo de user_cart incluido
</commit_message>
<xml_diff>
--- a/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
+++ b/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\DH\BierClub\entregas - sprints\6to-sprint (Base de Datos)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF9462A2-E041-4AF2-B592-92B608763148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B78F22C-B98E-45F8-A22F-BE5B8BFF2AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58F40C9B-E5F1-479F-9C1F-BC3593E56FF6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -84,30 +84,9 @@
     <t>IMAGES</t>
   </si>
   <si>
-    <t>Garu</t>
-  </si>
-  <si>
-    <t>Pepe</t>
-  </si>
-  <si>
     <t>producto 2</t>
   </si>
   <si>
-    <t>img1</t>
-  </si>
-  <si>
-    <t>img2</t>
-  </si>
-  <si>
-    <t>img3</t>
-  </si>
-  <si>
-    <t>img4</t>
-  </si>
-  <si>
-    <t>img5</t>
-  </si>
-  <si>
     <t>category_id(FK)</t>
   </si>
   <si>
@@ -166,13 +145,82 @@
   </si>
   <si>
     <t>cccc</t>
+  </si>
+  <si>
+    <t>USER_CART</t>
+  </si>
+  <si>
+    <t>Ippa Sippa</t>
+  </si>
+  <si>
+    <t>Saison Hoppy</t>
+  </si>
+  <si>
+    <t>William Scottish</t>
+  </si>
+  <si>
+    <t>Mumbai 1947</t>
+  </si>
+  <si>
+    <t>German Pills</t>
+  </si>
+  <si>
+    <t>producto 3</t>
+  </si>
+  <si>
+    <t>producto 4</t>
+  </si>
+  <si>
+    <t>producto 6</t>
+  </si>
+  <si>
+    <t>img1 - ippa</t>
+  </si>
+  <si>
+    <t>img2 - saison</t>
+  </si>
+  <si>
+    <t>img3 - ippa</t>
+  </si>
+  <si>
+    <t>img4 - ippa</t>
+  </si>
+  <si>
+    <t>img5 - german</t>
+  </si>
+  <si>
+    <t>img6 - mumbai</t>
+  </si>
+  <si>
+    <t>img7 - german</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>ivan @gmail.com</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>STATUS - CART</t>
+  </si>
+  <si>
+    <t>Sin compras</t>
+  </si>
+  <si>
+    <t>Carrito con productos</t>
+  </si>
+  <si>
+    <t>Carrito Finalizado (Ya comprado)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,8 +266,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +306,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,14 +335,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -276,9 +363,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Entrada" xfId="4" builtinId="20"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,15 +395,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -324,8 +418,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6819900" y="971550"/>
-          <a:ext cx="1181100" cy="1438275"/>
+          <a:off x="7581900" y="1533525"/>
+          <a:ext cx="1800225" cy="942975"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -351,13 +445,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -374,8 +468,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4257675" y="952500"/>
-          <a:ext cx="9525" cy="1485900"/>
+          <a:off x="4257676" y="1514475"/>
+          <a:ext cx="19049" cy="923925"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -453,13 +547,13 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -473,9 +567,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14020800" y="581025"/>
-          <a:ext cx="781050" cy="9525"/>
+        <a:xfrm flipV="1">
+          <a:off x="14820900" y="571500"/>
+          <a:ext cx="714375" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -550,16 +644,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -573,9 +667,59 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9420225" y="3467100"/>
-          <a:ext cx="2495550" cy="1724025"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13287375" y="3028951"/>
+          <a:ext cx="1990725" cy="1724024"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94AF0385-ADEC-45DB-B91E-E1BBF25A9424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10229850" y="5438775"/>
+          <a:ext cx="3810000" cy="28575"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -898,73 +1042,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF21648-E589-416D-B60E-7D410CC835E0}">
-  <dimension ref="E2:T30"/>
+  <dimension ref="E2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E2" s="2"/>
       <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="O2" s="1"/>
       <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="S2" s="3"/>
       <c r="T2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="G3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="K3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -973,10 +1111,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="H4" s="2">
         <v>10</v>
@@ -1003,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="5:20" x14ac:dyDescent="0.25">
@@ -1011,10 +1149,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -1023,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K5" s="2">
         <v>2</v>
@@ -1041,10 +1179,31 @@
         <v>2</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2">
+        <v>82</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>555</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
       <c r="O6" s="1">
         <v>3</v>
       </c>
@@ -1058,10 +1217,31 @@
         <v>3</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2">
+        <v>99</v>
+      </c>
+      <c r="H7" s="2">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
       <c r="O7" s="1">
         <v>4</v>
       </c>
@@ -1075,61 +1255,126 @@
         <v>4</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2">
+        <v>125</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5</v>
+      </c>
+      <c r="P8" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>6</v>
+      </c>
       <c r="S8" s="3">
         <v>5</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="O9" s="1">
+        <v>6</v>
+      </c>
+      <c r="P9" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>7</v>
+      </c>
+      <c r="S9" s="8">
+        <v>6</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="O10" s="1">
+        <v>7</v>
+      </c>
+      <c r="P10" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>5</v>
+      </c>
+      <c r="S10" s="8">
+        <v>7</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
       <c r="F14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="J14" s="1"/>
       <c r="K14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="N14" s="2"/>
+        <v>20</v>
+      </c>
       <c r="O14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="S14" s="12"/>
+      <c r="T14" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="2" t="s">
+      <c r="L15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="2" t="s">
+      <c r="O15" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="S15" s="12">
+        <v>0</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="5:20" x14ac:dyDescent="0.25">
@@ -1157,11 +1402,14 @@
       <c r="O16" s="2">
         <v>2</v>
       </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="S16" s="12">
+        <v>1</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
         <v>2</v>
       </c>
@@ -1184,13 +1432,16 @@
         <v>2</v>
       </c>
       <c r="O17" s="2">
-        <v>1</v>
-      </c>
-      <c r="P17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="S17" s="12">
+        <v>2</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
         <v>3</v>
       </c>
@@ -1213,55 +1464,106 @@
         <v>3</v>
       </c>
       <c r="O18" s="2">
-        <v>3</v>
-      </c>
-      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <v>4</v>
+      </c>
+      <c r="O19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <v>5</v>
+      </c>
+      <c r="O20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
+    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <v>6</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <v>7</v>
+      </c>
+      <c r="O22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <v>8</v>
+      </c>
+      <c r="O23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <v>9</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="2" t="s">
+      <c r="G27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="H28" s="2">
         <v>1234</v>
@@ -1273,18 +1575,27 @@
         <v>1</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1</v>
+      </c>
+      <c r="S28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E29" s="2">
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H29" s="2">
         <v>1234</v>
@@ -1296,18 +1607,27 @@
         <v>1</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2</v>
+      </c>
+      <c r="R29" s="1">
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E30" s="2">
         <v>3</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H30" s="2">
         <v>1234</v>
@@ -1319,7 +1639,103 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>3</v>
+      </c>
+      <c r="R30" s="1">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E31" s="2">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="2">
+        <v>34543</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>4</v>
+      </c>
+      <c r="R31" s="1">
+        <v>2</v>
+      </c>
+      <c r="S31" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1">
+        <v>5</v>
+      </c>
+      <c r="R32" s="1">
+        <v>2</v>
+      </c>
+      <c r="S32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="1">
+        <v>6</v>
+      </c>
+      <c r="R33" s="1">
+        <v>3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q34" s="1">
+        <v>7</v>
+      </c>
+      <c r="R34" s="1">
+        <v>4</v>
+      </c>
+      <c r="S34" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1">
+        <v>8</v>
+      </c>
+      <c r="R35" s="1">
+        <v>4</v>
+      </c>
+      <c r="S35" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1">
+        <v>9</v>
+      </c>
+      <c r="R36" s="1">
+        <v>4</v>
+      </c>
+      <c r="S36" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model de cart y user cambiados, agregado user_id
</commit_message>
<xml_diff>
--- a/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
+++ b/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\DH\BierClub\entregas - sprints\6to-sprint (Base de Datos)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A90526-9270-4831-A869-00C0A595ADD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4A5140-195E-4A6C-BDEE-4AAF42D3B0AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58F40C9B-E5F1-479F-9C1F-BC3593E56FF6}"/>
   </bookViews>
@@ -69,18 +69,9 @@
     <t>PC</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>IMAGE_PRODUCT</t>
   </si>
   <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t>image_id</t>
-  </si>
-  <si>
     <t>IMAGES</t>
   </si>
   <si>
@@ -90,18 +81,12 @@
     <t>category_id(FK)</t>
   </si>
   <si>
-    <t>cart_id</t>
-  </si>
-  <si>
     <t>CART_PRODUCT</t>
   </si>
   <si>
     <t>CARTS</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>USERS</t>
   </si>
   <si>
@@ -208,6 +193,21 @@
   </si>
   <si>
     <t>Carrito Con o Sin Productos</t>
+  </si>
+  <si>
+    <t>user_id(FK)</t>
+  </si>
+  <si>
+    <t>image_id(FK)</t>
+  </si>
+  <si>
+    <t>product_id(FK)</t>
+  </si>
+  <si>
+    <t>cart_id(FK)</t>
+  </si>
+  <si>
+    <t>id(PK)</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <dimension ref="E2:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,6 +997,8 @@
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
     <col min="20" max="20" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1005,16 +1007,16 @@
         <v>7</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="T2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E3" s="9" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>0</v>
@@ -1032,19 +1034,19 @@
         <v>4</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="T3" s="11" t="s">
         <v>0</v>
@@ -1055,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2">
         <v>90</v>
@@ -1085,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="5:20" x14ac:dyDescent="0.25">
@@ -1093,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2">
         <v>115</v>
@@ -1105,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K5" s="2">
         <v>2</v>
@@ -1123,7 +1125,7 @@
         <v>2</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="5:20" x14ac:dyDescent="0.25">
@@ -1131,7 +1133,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2">
         <v>82</v>
@@ -1143,7 +1145,7 @@
         <v>555</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -1161,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="5:20" x14ac:dyDescent="0.25">
@@ -1169,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2">
         <v>99</v>
@@ -1181,7 +1183,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K7" s="2">
         <v>2</v>
@@ -1199,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="5:20" x14ac:dyDescent="0.25">
@@ -1207,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2">
         <v>125</v>
@@ -1219,7 +1221,7 @@
         <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K8" s="2">
         <v>2</v>
@@ -1237,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="5:20" x14ac:dyDescent="0.25">
@@ -1254,7 +1256,7 @@
         <v>6</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="5:20" x14ac:dyDescent="0.25">
@@ -1271,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="5:20" x14ac:dyDescent="0.25">
@@ -1279,19 +1281,19 @@
         <v>6</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="S14" s="12"/>
       <c r="T14" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E15" s="9" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>0</v>
@@ -1300,28 +1302,28 @@
         <v>8</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="S15" s="12">
         <v>0</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="5:20" x14ac:dyDescent="0.25">
@@ -1356,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.25">
@@ -1485,30 +1487,30 @@
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F26" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27" s="9" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>0</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
@@ -1516,10 +1518,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="H28" s="2">
         <v>1234</v>
@@ -1531,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.25">
@@ -1539,10 +1541,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H29" s="2">
         <v>1234</v>
@@ -1554,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="5:16" x14ac:dyDescent="0.25">
@@ -1562,10 +1564,10 @@
         <v>3</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H30" s="2">
         <v>1234</v>
@@ -1577,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="5:16" x14ac:dyDescent="0.25">
@@ -1585,10 +1587,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H31" s="2">
         <v>34543</v>
@@ -1600,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
structure and data base updated
</commit_message>
<xml_diff>
--- a/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
+++ b/entregas - sprints/6to-sprint (Base de Datos)/excel-bierclub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\DH\BierClub\entregas - sprints\6to-sprint (Base de Datos)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D7DFCF-7F20-4BE4-848A-07F5B33A56FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D885A64-B71F-4EB7-827E-8B25BFB166F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58F40C9B-E5F1-479F-9C1F-BC3593E56FF6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>name</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Retiro en el local</t>
+  </si>
+  <si>
+    <t>stock_order</t>
   </si>
 </sst>
 </file>
@@ -275,14 +278,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -345,6 +340,14 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,24 +419,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -701,16 +704,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -724,9 +727,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8429625" y="3067050"/>
-          <a:ext cx="933450" cy="9525"/>
+        <a:xfrm>
+          <a:off x="9467850" y="3067050"/>
+          <a:ext cx="542925" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -760,16 +763,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>647701</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -784,8 +787,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7743825" y="3429000"/>
-          <a:ext cx="1524000" cy="1866900"/>
+          <a:off x="6781800" y="4267200"/>
+          <a:ext cx="3238501" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1117,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF21648-E589-416D-B60E-7D410CC835E0}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,9 +1132,11 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="15.28515625" customWidth="1"/>
@@ -1139,613 +1144,625 @@
     <col min="20" max="20" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="6" t="s">
+    <row r="2" spans="1:17" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>90</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>10</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>10</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+      <c r="M4" s="12">
         <v>2</v>
       </c>
-      <c r="O4" s="13">
-        <v>1</v>
-      </c>
-      <c r="P4" s="8" t="s">
+      <c r="O4" s="12">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="13">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="12">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>115</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>0</v>
       </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>2</v>
       </c>
-      <c r="L5" s="13">
-        <v>1</v>
-      </c>
-      <c r="M5" s="13">
+      <c r="L5" s="12">
+        <v>1</v>
+      </c>
+      <c r="M5" s="12">
         <v>3</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>2</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="13">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="12">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>82</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>5</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>555</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="9">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
         <v>3</v>
       </c>
-      <c r="L6" s="13">
-        <v>1</v>
-      </c>
-      <c r="M6" s="13">
+      <c r="L6" s="12">
+        <v>1</v>
+      </c>
+      <c r="M6" s="12">
         <v>4</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <v>3</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="13">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="12">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>99</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>20</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>10</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>2</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>4</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>2</v>
       </c>
-      <c r="M7" s="13">
-        <v>1</v>
-      </c>
-      <c r="O7" s="13">
+      <c r="M7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="12">
         <v>4</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="13">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="12">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>125</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>10</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>45</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>5</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <v>4</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>6</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="12">
         <v>5</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K9" s="8">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K9" s="7">
         <v>6</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="12">
         <v>5</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="12">
         <v>7</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="12">
         <v>6</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K10" s="8">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K10" s="7">
         <v>7</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="12">
         <v>5</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="12">
         <v>5</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="12">
         <v>7</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="D14" s="6" t="s">
+    <row r="14" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="D14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="M15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="N15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="O15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="10" t="s">
+      <c r="P15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="Q15" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
-      <c r="J16" s="13">
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7">
+        <v>5</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
         <v>2</v>
       </c>
-      <c r="L16" s="13">
-        <v>1</v>
-      </c>
-      <c r="M16" s="8">
-        <v>1</v>
-      </c>
-      <c r="N16" s="13">
-        <v>1</v>
-      </c>
-      <c r="O16" s="8">
+      <c r="M16" s="12">
+        <v>1</v>
+      </c>
+      <c r="N16" s="7">
+        <v>1</v>
+      </c>
+      <c r="O16" s="12">
+        <v>1</v>
+      </c>
+      <c r="P16" s="7">
         <v>0</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="Q16" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="13">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="8">
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7">
         <v>2</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
         <v>2</v>
       </c>
-      <c r="J17" s="13">
+      <c r="K17" s="12">
         <v>2</v>
       </c>
-      <c r="L17" s="13">
+      <c r="M17" s="12">
         <v>2</v>
       </c>
-      <c r="M17" s="8">
-        <v>1</v>
-      </c>
-      <c r="N17" s="13">
-        <v>1</v>
-      </c>
-      <c r="O17" s="8">
-        <v>1</v>
-      </c>
-      <c r="P17" s="8" t="s">
+      <c r="N17" s="7">
+        <v>1</v>
+      </c>
+      <c r="O17" s="12">
+        <v>1</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="13">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
         <v>3</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>0</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="7">
         <v>3</v>
       </c>
-      <c r="I18" s="13">
-        <v>1</v>
-      </c>
-      <c r="J18" s="13">
+      <c r="I18" s="7">
         <v>3</v>
       </c>
-      <c r="L18" s="13">
+      <c r="J18" s="12">
+        <v>1</v>
+      </c>
+      <c r="K18" s="12">
         <v>3</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="12">
+        <v>3</v>
+      </c>
+      <c r="N18" s="7">
         <v>0</v>
       </c>
-      <c r="N18" s="13">
-        <v>1</v>
-      </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="12">
+        <v>1</v>
+      </c>
+      <c r="P18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P18" s="8" t="s">
+      <c r="Q18" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L19" s="13">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M19" s="12">
         <v>4</v>
       </c>
-      <c r="M19" s="8">
-        <v>1</v>
-      </c>
-      <c r="N19" s="13">
+      <c r="N19" s="7">
+        <v>1</v>
+      </c>
+      <c r="O19" s="12">
         <v>2</v>
       </c>
-      <c r="O19" s="8">
-        <v>1</v>
-      </c>
-      <c r="P19" s="8" t="s">
+      <c r="P19" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L20" s="13">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M20" s="12">
         <v>5</v>
       </c>
-      <c r="M20" s="8">
+      <c r="N20" s="7">
         <v>0</v>
       </c>
-      <c r="N20" s="13">
+      <c r="O20" s="12">
         <v>2</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="P20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P20" s="8" t="s">
+      <c r="Q20" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="13">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M21" s="12">
         <v>6</v>
       </c>
-      <c r="M21" s="8">
+      <c r="N21" s="7">
         <v>0</v>
       </c>
-      <c r="N21" s="13">
+      <c r="O21" s="12">
         <v>3</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="P21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="Q21" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="13">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M22" s="12">
         <v>7</v>
       </c>
-      <c r="M22" s="8">
-        <v>1</v>
-      </c>
-      <c r="N22" s="13">
+      <c r="N22" s="7">
+        <v>1</v>
+      </c>
+      <c r="O22" s="12">
         <v>4</v>
       </c>
-      <c r="O22" s="8">
-        <v>1</v>
-      </c>
-      <c r="P22" s="8" t="s">
+      <c r="P22" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="13">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M23" s="12">
         <v>8</v>
       </c>
-      <c r="M23" s="8">
-        <v>1</v>
-      </c>
-      <c r="N23" s="13">
+      <c r="N23" s="7">
+        <v>1</v>
+      </c>
+      <c r="O23" s="12">
         <v>4</v>
       </c>
-      <c r="O23" s="8">
+      <c r="P23" s="7">
         <v>0</v>
       </c>
-      <c r="P23" s="8" t="s">
+      <c r="Q23" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="13">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M24" s="12">
         <v>9</v>
       </c>
-      <c r="M24" s="8">
+      <c r="N24" s="7">
         <v>0</v>
       </c>
-      <c r="N24" s="13">
+      <c r="O24" s="12">
         <v>4</v>
       </c>
-      <c r="O24" s="8" t="s">
+      <c r="P24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P24" s="8" t="s">
+      <c r="Q24" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="3:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="D26" s="6" t="s">
+    <row r="26" spans="3:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="D26" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="10" t="s">
+    <row r="27" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C28" s="13">
-        <v>1</v>
-      </c>
-      <c r="D28" s="8" t="s">
+    <row r="28" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="12">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>1234</v>
       </c>
-      <c r="G28" s="8">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1</v>
-      </c>
-      <c r="I28" s="8" t="s">
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>30</v>
       </c>
       <c r="M28" s="3"/>
-      <c r="N28" s="4" t="s">
+      <c r="N28" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C29" s="13">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="12">
         <v>2</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>1234</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <v>0</v>
       </c>
-      <c r="H29" s="8">
-        <v>1</v>
-      </c>
-      <c r="I29" s="8" t="s">
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>31</v>
       </c>
       <c r="M29" s="3">
@@ -1755,26 +1772,26 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="13">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="12">
         <v>3</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>1234</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <v>0</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="7">
         <v>0</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="M30" s="3">
@@ -1784,48 +1801,48 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C31" s="13">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="12">
         <v>4</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>34543</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="7">
         <v>0</v>
       </c>
-      <c r="H31" s="8">
-        <v>1</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="H31" s="7">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="32" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M32" s="3"/>
+      <c r="N32" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="33" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M33" s="3"/>
-      <c r="N33" s="4" t="s">
-        <v>62</v>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M35" s="3">
-        <v>1</v>
-      </c>
-      <c r="N35" s="3" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>